<commit_message>
new configuration with the new subnetting to allow more devices in each vlan
</commit_message>
<xml_diff>
--- a/configurations/subnetting-new.xlsx
+++ b/configurations/subnetting-new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\courses\DEPI-CISCO\lectures\project\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D1CF590-DBB5-4FB0-B1FC-12D45D5D0371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEB8B51-2878-4170-9CD7-260C85D2EB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{394C3ED4-B020-4617-837F-0240F49FB92B}"/>
+    <workbookView xWindow="12312" yWindow="708" windowWidth="10392" windowHeight="10224" xr2:uid="{394C3ED4-B020-4617-837F-0240F49FB92B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -100,9 +99,6 @@
     <t>Branch Subnetting (/24)</t>
   </si>
   <si>
-    <t>VLAN Subnetting (/27)</t>
-  </si>
-  <si>
     <t>VLAN Name</t>
   </si>
   <si>
@@ -173,6 +169,9 @@
   </si>
   <si>
     <t>192.168.1.225 - 192.168.1.254</t>
+  </si>
+  <si>
+    <t>VLAN Subnetting (/27)  .224</t>
   </si>
 </sst>
 </file>
@@ -240,10 +239,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -562,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C6ABC9-8EDD-4B6B-AD7C-9DC13D883A5C}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,11 +574,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -652,15 +651,15 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -674,83 +673,83 @@
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>11</v>

</xml_diff>